<commit_message>
Adding lib folder to store all jars and adding TestNG.xml in bin folder and adding TestNGrerun.xml in test output
</commit_message>
<xml_diff>
--- a/bin/testdata/TestData.xlsx
+++ b/bin/testdata/TestData.xlsx
@@ -9,17 +9,18 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1420" yWindow="10120" windowWidth="28800" windowHeight="6780" tabRatio="500" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="7280" windowWidth="28800" windowHeight="6780" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="loginWebVZFL" sheetId="5" r:id="rId1"/>
-    <sheet name="addPlaceTest" sheetId="1" r:id="rId2"/>
-    <sheet name="addContactsTest" sheetId="6" r:id="rId3"/>
-    <sheet name="addLBAlertWithPlaceTest" sheetId="4" r:id="rId4"/>
-    <sheet name="addLBAlertExistingPlaceTest" sheetId="7" r:id="rId5"/>
-    <sheet name="removePlaceTest" sheetId="9" r:id="rId6"/>
-    <sheet name="removeLBAlertTest" sheetId="8" r:id="rId7"/>
-    <sheet name="removeContactsTest " sheetId="12" r:id="rId8"/>
+    <sheet name="addPlaceTest (OLD)" sheetId="13" r:id="rId2"/>
+    <sheet name="addPlaceTest" sheetId="1" r:id="rId3"/>
+    <sheet name="addContactsTest" sheetId="6" r:id="rId4"/>
+    <sheet name="addLBAlertWithPlaceTest" sheetId="4" r:id="rId5"/>
+    <sheet name="addLBAlertExistingPlaceTest" sheetId="7" r:id="rId6"/>
+    <sheet name="removePlaceTest" sheetId="9" r:id="rId7"/>
+    <sheet name="removeLBAlertTest" sheetId="8" r:id="rId8"/>
+    <sheet name="removeContactsTest" sheetId="12" r:id="rId9"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="23">
   <si>
     <t>entersearchfield</t>
   </si>
@@ -467,7 +468,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -502,7 +503,7 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -568,10 +569,79 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="17.33203125" customWidth="1"/>
+    <col min="3" max="3" width="17.1640625" customWidth="1"/>
+    <col min="4" max="4" width="44.5" customWidth="1"/>
+    <col min="5" max="5" width="30.6640625" customWidth="1"/>
+    <col min="6" max="6" width="43" customWidth="1"/>
+    <col min="7" max="7" width="30.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+      <c r="A2" s="3">
+        <v>9493300677</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="C1" sqref="C1:C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -623,12 +693,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A2"/>
+      <selection activeCell="C2" sqref="C2:G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -717,7 +787,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G2"/>
   <sheetViews>
@@ -788,7 +858,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C2"/>
   <sheetViews>
@@ -829,7 +899,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C2"/>
   <sheetViews>
@@ -869,12 +939,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
updated to include case when theres no alerts and no places to delete.
</commit_message>
<xml_diff>
--- a/bin/testdata/TestData.xlsx
+++ b/bin/testdata/TestData.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28908"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="29005"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/atong/Documents/EclipseProjects/FamilyLocator/src/testdata/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/atong/Documents/EclipseProjects/FamilyLocator/bin/testdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="7280" windowWidth="28800" windowHeight="6780" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="1180" yWindow="10340" windowWidth="28800" windowHeight="6780" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="loginWebVZFL" sheetId="5" r:id="rId1"/>
@@ -52,9 +52,6 @@
     <t>placename</t>
   </si>
   <si>
-    <t>5521 Alton</t>
-  </si>
-  <si>
     <t>5521 Alton Pkwy, Irvine, CA 92618, USA</t>
   </si>
   <si>
@@ -103,11 +100,14 @@
     <t>nimtester00@gmail.com</t>
   </si>
   <si>
-    <t>14201 Jeffrey</t>
-  </si>
-  <si>
     <t>14201 Jeffrey Rd
 Irvine, CA 92620</t>
+  </si>
+  <si>
+    <t>14201 Jeffrey Rd, Irvine, CA</t>
+  </si>
+  <si>
+    <t>5521 Alton Pkwy, Irvine, CA</t>
   </si>
 </sst>
 </file>
@@ -479,10 +479,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" t="s">
         <v>8</v>
-      </c>
-      <c r="B1" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -490,7 +490,7 @@
         <v>9493300677</v>
       </c>
       <c r="B2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -503,13 +503,13 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="17.33203125" customWidth="1"/>
-    <col min="3" max="3" width="17.1640625" customWidth="1"/>
+    <col min="3" max="3" width="26.6640625" customWidth="1"/>
     <col min="4" max="4" width="44.5" customWidth="1"/>
     <col min="5" max="5" width="30.6640625" customWidth="1"/>
     <col min="6" max="6" width="43" customWidth="1"/>
@@ -518,10 +518,10 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>9</v>
       </c>
       <c r="C1" t="s">
         <v>0</v>
@@ -544,22 +544,22 @@
         <v>9493300677</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C2" t="s">
+      <c r="E2" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>6</v>
-      </c>
-      <c r="G2" t="s">
-        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -578,7 +578,7 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="17.33203125" customWidth="1"/>
-    <col min="3" max="3" width="17.1640625" customWidth="1"/>
+    <col min="3" max="3" width="36.33203125" customWidth="1"/>
     <col min="4" max="4" width="44.5" customWidth="1"/>
     <col min="5" max="5" width="30.6640625" customWidth="1"/>
     <col min="6" max="6" width="43" customWidth="1"/>
@@ -587,10 +587,10 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>9</v>
       </c>
       <c r="C1" t="s">
         <v>0</v>
@@ -613,22 +613,22 @@
         <v>9493300677</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C2" t="s">
         <v>21</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E2" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" t="s">
         <v>14</v>
-      </c>
-      <c r="F2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G2" t="s">
-        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -653,19 +653,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" t="s">
         <v>8</v>
       </c>
-      <c r="B1" t="s">
-        <v>9</v>
-      </c>
       <c r="C1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" t="s">
         <v>16</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>17</v>
-      </c>
-      <c r="E1" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -673,16 +673,16 @@
         <v>9493300677</v>
       </c>
       <c r="B2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2">
+        <v>9493300677</v>
+      </c>
+      <c r="E2" s="5" t="s">
         <v>19</v>
-      </c>
-      <c r="D2">
-        <v>9493300677</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -698,14 +698,14 @@
   <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:G2"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="15" customWidth="1"/>
     <col min="2" max="2" width="13.83203125" customWidth="1"/>
-    <col min="3" max="3" width="17.1640625" customWidth="1"/>
+    <col min="3" max="3" width="26.83203125" customWidth="1"/>
     <col min="4" max="4" width="25.83203125" customWidth="1"/>
     <col min="5" max="5" width="41" customWidth="1"/>
     <col min="6" max="6" width="43" customWidth="1"/>
@@ -717,10 +717,10 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>9</v>
       </c>
       <c r="C1" t="s">
         <v>0</v>
@@ -738,13 +738,13 @@
         <v>4</v>
       </c>
       <c r="H1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I1" t="s">
         <v>16</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>17</v>
-      </c>
-      <c r="J1" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="32" x14ac:dyDescent="0.2">
@@ -752,31 +752,31 @@
         <v>9493300677</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C2" t="s">
         <v>21</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E2" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" t="s">
         <v>14</v>
       </c>
-      <c r="F2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G2" t="s">
-        <v>15</v>
-      </c>
       <c r="H2" t="s">
+        <v>18</v>
+      </c>
+      <c r="I2">
+        <v>9493300677</v>
+      </c>
+      <c r="J2" s="5" t="s">
         <v>19</v>
-      </c>
-      <c r="I2">
-        <v>9493300677</v>
-      </c>
-      <c r="J2" s="5" t="s">
-        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -798,7 +798,7 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="2" width="17.1640625" customWidth="1"/>
-    <col min="3" max="3" width="15.33203125" customWidth="1"/>
+    <col min="3" max="3" width="33.83203125" customWidth="1"/>
     <col min="4" max="4" width="11.6640625" customWidth="1"/>
     <col min="5" max="5" width="15.5" customWidth="1"/>
     <col min="6" max="6" width="21.5" customWidth="1"/>
@@ -806,10 +806,10 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>9</v>
       </c>
       <c r="C1" t="s">
         <v>3</v>
@@ -818,13 +818,13 @@
         <v>4</v>
       </c>
       <c r="E1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1" t="s">
         <v>16</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>17</v>
-      </c>
-      <c r="G1" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
@@ -832,22 +832,22 @@
         <v>9493300677</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2">
+        <v>9493300677</v>
+      </c>
+      <c r="G2" s="5" t="s">
         <v>19</v>
-      </c>
-      <c r="F2">
-        <v>9493300677</v>
-      </c>
-      <c r="G2" s="5" t="s">
-        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -874,10 +874,10 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>9</v>
       </c>
       <c r="C1" t="s">
         <v>4</v>
@@ -888,10 +888,10 @@
         <v>9493300677</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -914,10 +914,10 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>9</v>
       </c>
       <c r="C1" t="s">
         <v>4</v>
@@ -928,10 +928,10 @@
         <v>9493300677</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -954,10 +954,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="6" t="s">
         <v>8</v>
-      </c>
-      <c r="B1" s="6" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -965,7 +965,7 @@
         <v>9493300677</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added scheduled alert test
</commit_message>
<xml_diff>
--- a/bin/testdata/TestData.xlsx
+++ b/bin/testdata/TestData.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/atong/Documents/EclipseProjects/FamilyLocator/bin/testdata/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/atong/Documents/EclipseProjects/FamilyLocator/src/testdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1180" yWindow="10340" windowWidth="28800" windowHeight="6780" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="3340" windowWidth="28800" windowHeight="8660" tabRatio="500" firstSheet="2" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="loginWebVZFL" sheetId="5" r:id="rId1"/>
@@ -21,6 +21,8 @@
     <sheet name="removePlaceTest" sheetId="9" r:id="rId7"/>
     <sheet name="removeLBAlertTest" sheetId="8" r:id="rId8"/>
     <sheet name="removeContactsTest" sheetId="12" r:id="rId9"/>
+    <sheet name="addSchedAlertTest" sheetId="14" r:id="rId10"/>
+    <sheet name="removeSchedAlertTest" sheetId="15" r:id="rId11"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -35,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="28">
   <si>
     <t>entersearchfield</t>
   </si>
@@ -108,6 +110,21 @@
   </si>
   <si>
     <t>5521 Alton Pkwy, Irvine, CA</t>
+  </si>
+  <si>
+    <t>reviewschedalerttime</t>
+  </si>
+  <si>
+    <t>schedalerttime</t>
+  </si>
+  <si>
+    <t>addedschedalert</t>
+  </si>
+  <si>
+    <t>2:00 PM Pacific</t>
+  </si>
+  <si>
+    <t>schedalerttoremove</t>
   </si>
 </sst>
 </file>
@@ -171,7 +188,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -181,6 +198,12 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="5"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="5" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="18" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
@@ -498,6 +521,128 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I1" sqref="I1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="14.1640625" style="6" customWidth="1"/>
+    <col min="2" max="2" width="12.6640625" style="6" customWidth="1"/>
+    <col min="3" max="3" width="18.33203125" style="6" customWidth="1"/>
+    <col min="4" max="4" width="14.6640625" style="6" customWidth="1"/>
+    <col min="5" max="5" width="26.33203125" style="6" customWidth="1"/>
+    <col min="6" max="6" width="13.1640625" style="6" customWidth="1"/>
+    <col min="7" max="7" width="25" customWidth="1"/>
+    <col min="8" max="8" width="22.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" s="6">
+        <v>9493300677</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" s="6">
+        <v>9493300677</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="F2" s="8">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E2" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="14.1640625" style="6" customWidth="1"/>
+    <col min="2" max="2" width="12.6640625" style="6" customWidth="1"/>
+    <col min="3" max="3" width="18.33203125" style="6" customWidth="1"/>
+    <col min="12" max="12" width="16" customWidth="1"/>
+    <col min="14" max="14" width="19.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="6">
+        <v>9493300677</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G2"/>
@@ -571,7 +716,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
@@ -641,14 +786,16 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C2"/>
+      <selection activeCell="C1" sqref="C1:E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="16.33203125" customWidth="1"/>
     <col min="2" max="2" width="14.83203125" customWidth="1"/>
-    <col min="3" max="3" width="25.5" customWidth="1"/>
+    <col min="3" max="3" width="19.33203125" customWidth="1"/>
+    <col min="4" max="4" width="15.83203125" customWidth="1"/>
+    <col min="5" max="5" width="28.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
@@ -698,7 +845,7 @@
   <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="H1" sqref="H1:J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -944,7 +1091,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B2" sqref="A1:B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>